<commit_message>
fix date read for sax bug
</commit_message>
<xml_diff>
--- a/hutool-poi/src/test/resources/data_for_sax_test.xlsx
+++ b/hutool-poi/src/test/resources/data_for_sax_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\java\looly\hutool\hutool-poi\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37F5D5AB-6414-4E60-A53A-529F6B94B3A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B468A1B5-F875-4908-AAD8-822007128B2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11746"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11746" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="179" formatCode="#,##0.00;[Red]#,##0.00"/>
+    <numFmt numFmtId="177" formatCode="#,##0.00;[Red]#,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -74,17 +74,20 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="31" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -400,16 +403,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.1328125" customWidth="1"/>
+    <col min="1" max="1" width="19.06640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
@@ -437,6 +440,11 @@
       <c r="B4">
         <f>ROUND(A4 * 0.05,3)</f>
         <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" s="4">
+        <v>41264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>